<commit_message>
minor corrections, but working well
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="380" windowWidth="11040" windowHeight="12920" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="5080" windowWidth="24520" windowHeight="9340" tabRatio="385"/>
   </bookViews>
   <sheets>
     <sheet name="FiveStates" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="96">
   <si>
     <t>dhID</t>
   </si>
@@ -142,9 +142,6 @@
     <t>votecount_dupage</t>
   </si>
   <si>
-    <t>votepct_dupage</t>
-  </si>
-  <si>
     <t>totalvotes_dupage</t>
   </si>
   <si>
@@ -265,33 +262,6 @@
     <t>pct.</t>
   </si>
   <si>
-    <t>DUPAGE</t>
-  </si>
-  <si>
-    <t>KANE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAKE </t>
-  </si>
-  <si>
-    <t>MCHENRY</t>
-  </si>
-  <si>
-    <t>WILL</t>
-  </si>
-  <si>
-    <t>CHICAGO</t>
-  </si>
-  <si>
-    <t>STATEWIDE</t>
-  </si>
-  <si>
-    <t>precntstotal</t>
-  </si>
-  <si>
-    <t>SubCook prrep</t>
-  </si>
-  <si>
     <t>#chi precents:</t>
   </si>
   <si>
@@ -314,6 +284,30 @@
   </si>
   <si>
     <t>Delegates at stake:</t>
+  </si>
+  <si>
+    <t>precinctsreporting</t>
+  </si>
+  <si>
+    <t>precinctstotal</t>
+  </si>
+  <si>
+    <t>precinctsreportingpct_kane</t>
+  </si>
+  <si>
+    <t>precinctsreportingpct_lake</t>
+  </si>
+  <si>
+    <t>precinctsreportingpct_mch</t>
+  </si>
+  <si>
+    <t>precinctsreportingpct_will</t>
+  </si>
+  <si>
+    <t>precinctsreportingpct_chi</t>
+  </si>
+  <si>
+    <t>precinctsreportingpct_statewide</t>
   </si>
 </sst>
 </file>
@@ -383,8 +377,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,7 +474,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -509,6 +511,10 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -545,6 +551,10 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -877,8 +887,8 @@
   <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="7" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -895,7 +905,7 @@
     <col min="10" max="10" width="7.83203125" customWidth="1"/>
     <col min="12" max="12" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -963,34 +973,34 @@
         <v>17</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
+        <v>33.1</v>
       </c>
       <c r="G2">
-        <v>0.2</v>
+        <v>0.52546899999999996</v>
       </c>
       <c r="H2">
-        <v>0.8</v>
+        <v>40.26</v>
       </c>
       <c r="I2">
-        <v>0.9</v>
+        <v>0.57988099999999998</v>
       </c>
       <c r="J2">
-        <v>0.15</v>
+        <v>52.64</v>
       </c>
       <c r="K2">
-        <v>0.16</v>
+        <v>0.55441200000000002</v>
       </c>
       <c r="L2">
-        <v>0.22</v>
+        <v>16.21</v>
       </c>
       <c r="M2">
-        <v>0.23</v>
+        <v>0.48092699999999999</v>
       </c>
       <c r="N2">
-        <v>0.28999999999999998</v>
+        <v>95.94</v>
       </c>
       <c r="O2">
-        <v>0.3</v>
+        <v>0.644845</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1010,34 +1020,34 @@
         <v>17</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>33.1</v>
       </c>
       <c r="G3">
-        <v>0.3</v>
+        <v>0.46599000000000002</v>
       </c>
       <c r="H3">
-        <v>0.8</v>
+        <v>40.26</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
+        <v>0.41008099999999997</v>
       </c>
       <c r="J3">
-        <v>0.15</v>
+        <v>52.64</v>
       </c>
       <c r="K3">
-        <v>0.17</v>
+        <v>0.40234900000000001</v>
       </c>
       <c r="L3">
-        <v>0.22</v>
+        <v>16.21</v>
       </c>
       <c r="M3">
-        <v>0.24</v>
+        <v>0.49974099999999999</v>
       </c>
       <c r="N3">
-        <v>0.28999999999999998</v>
+        <v>95.94</v>
       </c>
       <c r="O3">
-        <v>0.31</v>
+        <v>0.33213900000000002</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1057,34 +1067,34 @@
         <v>22</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>32.28</v>
       </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>0.40168799999999999</v>
       </c>
       <c r="H4">
-        <v>0.8</v>
+        <v>40.090000000000003</v>
       </c>
       <c r="I4">
-        <v>0.11</v>
+        <v>0.36869200000000002</v>
       </c>
       <c r="J4">
-        <v>0.15</v>
+        <v>52.34</v>
       </c>
       <c r="K4">
-        <v>0.18</v>
+        <v>0.40190999999999999</v>
       </c>
       <c r="L4">
-        <v>0.22</v>
+        <v>16.21</v>
       </c>
       <c r="M4">
-        <v>0.25</v>
+        <v>0.42666700000000002</v>
       </c>
       <c r="N4">
-        <v>0.28999999999999998</v>
+        <v>95.94</v>
       </c>
       <c r="O4">
-        <v>0.32</v>
+        <v>0.45726099999999997</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1104,34 +1114,34 @@
         <v>22</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>32.28</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>0.25918200000000002</v>
       </c>
       <c r="H5">
-        <v>0.8</v>
+        <v>40.090000000000003</v>
       </c>
       <c r="I5">
-        <v>0.12</v>
+        <v>0.145403</v>
       </c>
       <c r="J5">
-        <v>0.15</v>
+        <v>52.34</v>
       </c>
       <c r="K5">
-        <v>0.19</v>
+        <v>0.36409900000000001</v>
       </c>
       <c r="L5">
-        <v>0.22</v>
+        <v>16.21</v>
       </c>
       <c r="M5">
-        <v>0.26</v>
+        <v>0.40337200000000001</v>
       </c>
       <c r="N5">
-        <v>0.28999999999999998</v>
+        <v>95.94</v>
       </c>
       <c r="O5">
-        <v>0.33</v>
+        <v>0.17090900000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1151,34 +1161,34 @@
         <v>22</v>
       </c>
       <c r="F6">
-        <v>0.1</v>
+        <v>32.28</v>
       </c>
       <c r="G6">
-        <v>0.6</v>
+        <v>9.4118999999999994E-2</v>
       </c>
       <c r="H6">
-        <v>0.8</v>
+        <v>40.090000000000003</v>
       </c>
       <c r="I6">
-        <v>0.13</v>
+        <v>2.9225000000000001E-2</v>
       </c>
       <c r="J6">
-        <v>0.15</v>
+        <v>52.34</v>
       </c>
       <c r="K6">
-        <v>0.2</v>
+        <v>8.2765000000000005E-2</v>
       </c>
       <c r="L6">
-        <v>0.22</v>
+        <v>16.21</v>
       </c>
       <c r="M6">
-        <v>0.27</v>
+        <v>5.9552000000000001E-2</v>
       </c>
       <c r="N6">
-        <v>0.28999999999999998</v>
+        <v>95.94</v>
       </c>
       <c r="O6">
-        <v>0.34</v>
+        <v>0.269816</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1198,34 +1208,34 @@
         <v>22</v>
       </c>
       <c r="F7">
-        <v>0.1</v>
+        <v>32.28</v>
       </c>
       <c r="G7">
-        <v>0.7</v>
+        <v>0.222749</v>
       </c>
       <c r="H7">
-        <v>0.8</v>
+        <v>40.090000000000003</v>
       </c>
       <c r="I7">
-        <v>0.14000000000000001</v>
+        <v>0.43782700000000002</v>
       </c>
       <c r="J7">
-        <v>0.15</v>
+        <v>52.34</v>
       </c>
       <c r="K7">
-        <v>0.21</v>
+        <v>0.12470299999999999</v>
       </c>
       <c r="L7">
-        <v>0.22</v>
+        <v>16.21</v>
       </c>
       <c r="M7">
-        <v>0.28000000000000003</v>
+        <v>7.9303999999999999E-2</v>
       </c>
       <c r="N7">
-        <v>0.28999999999999998</v>
+        <v>95.94</v>
       </c>
       <c r="O7">
-        <v>0.35</v>
+        <v>6.7677000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1233,13 +1243,13 @@
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2">
         <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1247,8 +1257,8 @@
         <v>29</v>
       </c>
       <c r="C12" s="4">
-        <f>F2</f>
-        <v>0.1</v>
+        <f>SUM(F2*0.01)</f>
+        <v>0.33100000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1257,7 +1267,7 @@
       </c>
       <c r="C13" s="4">
         <f>G2</f>
-        <v>0.2</v>
+        <v>0.52546899999999996</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1266,7 +1276,7 @@
       </c>
       <c r="C14" s="4">
         <f>G3</f>
-        <v>0.3</v>
+        <v>0.46599000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1275,18 +1285,18 @@
       </c>
       <c r="C15" s="4">
         <f>SUM(1-(C13+C14))</f>
-        <v>0.5</v>
+        <v>8.5410000000000208E-3</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="B16" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C16" s="9">
         <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1294,8 +1304,8 @@
         <v>32</v>
       </c>
       <c r="C17" s="4">
-        <f>F4</f>
-        <v>0.1</v>
+        <f>SUM(F4*0.01)</f>
+        <v>0.32280000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1304,7 +1314,7 @@
       </c>
       <c r="C18" s="4">
         <f>G4</f>
-        <v>0.4</v>
+        <v>0.40168799999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1313,7 +1323,7 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" ref="C19:C21" si="0">G5</f>
-        <v>0.5</v>
+        <v>0.25918200000000002</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1322,7 +1332,7 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>9.4118999999999994E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1331,7 +1341,7 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0.222749</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1340,7 +1350,7 @@
       </c>
       <c r="C22" s="4">
         <f>SUM(1-SUM(C18:C21))</f>
-        <v>-1.2000000000000002</v>
+        <v>2.2262000000000004E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1348,13 +1358,13 @@
         <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2">
         <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1362,8 +1372,8 @@
         <v>29</v>
       </c>
       <c r="C24" s="4">
-        <f>H2</f>
-        <v>0.8</v>
+        <f>SUM(H2*0.01)</f>
+        <v>0.40260000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1372,7 +1382,7 @@
       </c>
       <c r="C25" s="4">
         <f>I2</f>
-        <v>0.9</v>
+        <v>0.57988099999999998</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1381,7 +1391,7 @@
       </c>
       <c r="C26" s="4">
         <f>I3</f>
-        <v>0.1</v>
+        <v>0.41008099999999997</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1390,18 +1400,18 @@
       </c>
       <c r="C27" s="4">
         <f>SUM(1-(C25+C26))</f>
-        <v>0</v>
+        <v>1.0037999999999991E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="B28" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2">
         <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1409,8 +1419,8 @@
         <v>32</v>
       </c>
       <c r="C29" s="4">
-        <f>H4</f>
-        <v>0.8</v>
+        <f>SUM(H4*0.01)</f>
+        <v>0.40090000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1419,7 +1429,7 @@
       </c>
       <c r="C30" s="4">
         <f>I4</f>
-        <v>0.11</v>
+        <v>0.36869200000000002</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1428,7 +1438,7 @@
       </c>
       <c r="C31" s="4">
         <f t="shared" ref="C31:C33" si="1">I5</f>
-        <v>0.12</v>
+        <v>0.145403</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1437,7 +1447,7 @@
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>0.13</v>
+        <v>2.9225000000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1446,7 +1456,7 @@
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <v>0.43782700000000002</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1455,7 +1465,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(1-SUM(C30:C33))</f>
-        <v>0.5</v>
+        <v>1.8853000000000009E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1463,13 +1473,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2">
         <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1477,8 +1487,8 @@
         <v>29</v>
       </c>
       <c r="C36" s="4">
-        <f>J2</f>
-        <v>0.15</v>
+        <f>SUM(J2*0.01)</f>
+        <v>0.52639999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1487,7 +1497,7 @@
       </c>
       <c r="C37" s="4">
         <f>K2</f>
-        <v>0.16</v>
+        <v>0.55441200000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1496,7 +1506,7 @@
       </c>
       <c r="C38" s="4">
         <f>K3</f>
-        <v>0.17</v>
+        <v>0.40234900000000001</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1505,18 +1515,18 @@
       </c>
       <c r="C39" s="4">
         <f>SUM(1-(C37+C38))</f>
-        <v>0.66999999999999993</v>
+        <v>4.3239000000000027E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="B40" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C40" s="2">
         <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1524,8 +1534,8 @@
         <v>32</v>
       </c>
       <c r="C41" s="4">
-        <f>J4</f>
-        <v>0.15</v>
+        <f>SUM(J4*0.01)</f>
+        <v>0.52340000000000009</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1534,7 +1544,7 @@
       </c>
       <c r="C42" s="4">
         <f>K4</f>
-        <v>0.18</v>
+        <v>0.40190999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1543,7 +1553,7 @@
       </c>
       <c r="C43" s="4">
         <f t="shared" ref="C43:C45" si="2">K5</f>
-        <v>0.19</v>
+        <v>0.36409900000000001</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1552,7 +1562,7 @@
       </c>
       <c r="C44" s="4">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>8.2765000000000005E-2</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1561,7 +1571,7 @@
       </c>
       <c r="C45" s="4">
         <f t="shared" si="2"/>
-        <v>0.21</v>
+        <v>0.12470299999999999</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1570,7 +1580,7 @@
       </c>
       <c r="C46" s="4">
         <f>SUM(1-SUM(C42:C45))</f>
-        <v>0.21999999999999997</v>
+        <v>2.6523000000000074E-2</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1578,7 +1588,7 @@
         <v>35</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C47" s="2">
         <v>71</v>
@@ -1590,8 +1600,8 @@
         <v>29</v>
       </c>
       <c r="C48" s="4">
-        <f>L2</f>
-        <v>0.22</v>
+        <f>SUM(L2*0.01)</f>
+        <v>0.16210000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1601,7 +1611,7 @@
       </c>
       <c r="C49" s="4">
         <f>M2</f>
-        <v>0.23</v>
+        <v>0.48092699999999999</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1611,7 +1621,7 @@
       </c>
       <c r="C50" s="4">
         <f>M3</f>
-        <v>0.24</v>
+        <v>0.49974099999999999</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1621,19 +1631,19 @@
       </c>
       <c r="C51" s="4">
         <f>SUM(1-(C49+C50))</f>
-        <v>0.53</v>
+        <v>1.9332000000000016E-2</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1"/>
       <c r="B52" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C52" s="2">
         <v>52</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1642,8 +1652,8 @@
         <v>32</v>
       </c>
       <c r="C53" s="4">
-        <f>L4</f>
-        <v>0.22</v>
+        <f>SUM(L4*0.01)</f>
+        <v>0.16210000000000002</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1653,7 +1663,7 @@
       </c>
       <c r="C54" s="4">
         <f>M4</f>
-        <v>0.25</v>
+        <v>0.42666700000000002</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1663,7 +1673,7 @@
       </c>
       <c r="C55" s="4">
         <f t="shared" ref="C55:C57" si="3">M5</f>
-        <v>0.26</v>
+        <v>0.40337200000000001</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1673,7 +1683,7 @@
       </c>
       <c r="C56" s="4">
         <f t="shared" si="3"/>
-        <v>0.27</v>
+        <v>5.9552000000000001E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1683,7 +1693,7 @@
       </c>
       <c r="C57" s="4">
         <f t="shared" si="3"/>
-        <v>0.28000000000000003</v>
+        <v>7.9303999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1693,7 +1703,7 @@
       </c>
       <c r="C58" s="4">
         <f>SUM(1-SUM(C54:C57))</f>
-        <v>-6.0000000000000053E-2</v>
+        <v>3.1104999999999938E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1701,13 +1711,13 @@
         <v>36</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C59" s="2">
         <v>214</v>
       </c>
       <c r="D59" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1716,8 +1726,8 @@
         <v>29</v>
       </c>
       <c r="C60" s="4">
-        <f>N2</f>
-        <v>0.28999999999999998</v>
+        <f>SUM(N2*0.01)</f>
+        <v>0.95940000000000003</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1727,7 +1737,7 @@
       </c>
       <c r="C61" s="4">
         <f>O2</f>
-        <v>0.3</v>
+        <v>0.644845</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1737,7 +1747,7 @@
       </c>
       <c r="C62" s="4">
         <f>O3</f>
-        <v>0.31</v>
+        <v>0.33213900000000002</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1747,19 +1757,19 @@
       </c>
       <c r="C63" s="4">
         <f>SUM(1-(C61+C62))</f>
-        <v>0.39</v>
+        <v>2.3015999999999925E-2</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1"/>
       <c r="B64" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C64" s="2">
         <v>99</v>
       </c>
       <c r="D64" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1768,8 +1778,8 @@
         <v>32</v>
       </c>
       <c r="C65" s="4">
-        <f>N4</f>
-        <v>0.28999999999999998</v>
+        <f>SUM(N4*0.01)</f>
+        <v>0.95940000000000003</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1779,7 +1789,7 @@
       </c>
       <c r="C66" s="4">
         <f>O4</f>
-        <v>0.32</v>
+        <v>0.45726099999999997</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1789,7 +1799,7 @@
       </c>
       <c r="C67" s="4">
         <f t="shared" ref="C67:C69" si="4">O5</f>
-        <v>0.33</v>
+        <v>0.17090900000000001</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1799,7 +1809,7 @@
       </c>
       <c r="C68" s="4">
         <f t="shared" si="4"/>
-        <v>0.34</v>
+        <v>0.269816</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1809,7 +1819,7 @@
       </c>
       <c r="C69" s="4">
         <f t="shared" si="4"/>
-        <v>0.35</v>
+        <v>6.7677000000000001E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1819,7 +1829,7 @@
       </c>
       <c r="C70" s="4">
         <f>SUM(1-SUM(C66:C69))</f>
-        <v>-0.33999999999999986</v>
+        <v>3.4337000000000062E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1837,9 +1847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1849,20 +1859,20 @@
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" customWidth="1"/>
     <col min="15" max="15" width="9.1640625" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="17" width="9.5" customWidth="1"/>
-    <col min="18" max="18" width="6.1640625" customWidth="1"/>
-    <col min="19" max="19" width="9.83203125" customWidth="1"/>
+    <col min="18" max="18" width="24" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" customWidth="1"/>
     <col min="20" max="20" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.6640625" customWidth="1"/>
     <col min="22" max="22" width="9.5" bestFit="1" customWidth="1"/>
@@ -1899,214 +1909,214 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>89</v>
+      <c r="F1" t="s">
+        <v>88</v>
       </c>
       <c r="G1" t="s">
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>81</v>
+      <c r="J1" t="s">
+        <v>5</v>
       </c>
       <c r="K1" t="s">
         <v>39</v>
       </c>
       <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S1" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE1" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>55</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI1" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>10001</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2">
-        <v>300</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="F2">
+        <v>2547</v>
+      </c>
+      <c r="G2">
+        <v>415579</v>
+      </c>
+      <c r="H2">
         <v>3668</v>
       </c>
-      <c r="I2" s="2">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="M2" s="2">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O2" s="2">
-        <v>2</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>24</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="S2" s="2">
-        <v>2</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="U2" s="2">
-        <v>24</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="W2" s="2">
-        <v>2</v>
-      </c>
-      <c r="X2" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>24</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>14</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>24</v>
+      <c r="I2">
+        <v>776100</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>4509</v>
+      </c>
+      <c r="L2">
+        <v>0.51460899999999998</v>
+      </c>
+      <c r="M2">
+        <v>8762</v>
+      </c>
+      <c r="N2">
+        <v>24.58</v>
+      </c>
+      <c r="O2">
+        <v>4285</v>
+      </c>
+      <c r="P2">
+        <v>0.48593799999999998</v>
+      </c>
+      <c r="Q2">
+        <v>8818</v>
+      </c>
+      <c r="R2">
+        <v>8.92</v>
+      </c>
+      <c r="S2">
+        <v>28074</v>
+      </c>
+      <c r="T2">
+        <v>0.50611099999999998</v>
+      </c>
+      <c r="U2">
+        <v>55470</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0.73078782020299604</v>
+      </c>
+      <c r="AE2">
+        <v>267725</v>
+      </c>
+      <c r="AF2">
+        <v>0.53836903691816995</v>
+      </c>
+      <c r="AG2">
+        <v>497289</v>
+      </c>
+      <c r="AH2">
+        <v>33.1</v>
+      </c>
+      <c r="AI2">
+        <v>482862</v>
+      </c>
+      <c r="AJ2">
+        <v>0.52546899999999996</v>
+      </c>
+      <c r="AK2">
+        <v>918916</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -2125,214 +2135,214 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2">
-        <v>300</v>
+      <c r="F3">
+        <v>2547</v>
       </c>
       <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2">
+        <v>353746</v>
+      </c>
+      <c r="H3">
         <v>3668</v>
       </c>
       <c r="I3">
-        <v>24</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.1</v>
+        <v>776100</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>4228</v>
       </c>
       <c r="L3">
-        <v>0.14000000000000001</v>
+        <v>0.48253800000000002</v>
       </c>
       <c r="M3">
-        <v>24</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.1</v>
+        <v>8762</v>
+      </c>
+      <c r="N3">
+        <v>24.58</v>
       </c>
       <c r="O3">
-        <v>3</v>
+        <v>4503</v>
       </c>
       <c r="P3">
-        <v>0.14000000000000001</v>
+        <v>0.51066</v>
       </c>
       <c r="Q3">
-        <v>24</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0.1</v>
+        <v>8818</v>
+      </c>
+      <c r="R3">
+        <v>8.92</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>27227</v>
       </c>
       <c r="T3">
-        <v>0.14000000000000001</v>
+        <v>0.490842</v>
       </c>
       <c r="U3">
-        <v>24</v>
-      </c>
-      <c r="V3" s="2">
-        <v>0.1</v>
+        <v>55470</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>24</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>24</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE3">
+        <v>224469</v>
+      </c>
+      <c r="AF3">
+        <v>0.451385411702249</v>
+      </c>
+      <c r="AG3">
+        <v>497289</v>
+      </c>
+      <c r="AH3">
+        <v>33.1</v>
+      </c>
+      <c r="AI3">
+        <v>428206</v>
+      </c>
+      <c r="AJ3">
+        <v>0.46599000000000002</v>
+      </c>
+      <c r="AK3">
+        <v>918916</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" s="2" customFormat="1">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="AF3">
-        <v>0.12</v>
-      </c>
-      <c r="AG3">
-        <v>14</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AI3">
-        <v>3</v>
-      </c>
-      <c r="AJ3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="AK3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" s="2" customFormat="1">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>163003</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2">
-        <v>300</v>
-      </c>
-      <c r="G4" s="2">
-        <v>4</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="F4">
+        <v>2547</v>
+      </c>
+      <c r="G4">
+        <v>88809</v>
+      </c>
+      <c r="H4">
         <v>3668</v>
       </c>
-      <c r="I4" s="2">
-        <v>25</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>4</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="M4" s="2">
-        <v>25</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O4" s="2">
-        <v>4</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>25</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="S4" s="2">
-        <v>4</v>
-      </c>
-      <c r="T4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="U4" s="2">
-        <v>25</v>
-      </c>
-      <c r="V4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="W4" s="2">
-        <v>4</v>
-      </c>
-      <c r="X4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>25</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>25</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>3</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>25</v>
-      </c>
-      <c r="AH4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AI4" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="AK4" s="2">
-        <v>25</v>
+      <c r="I4">
+        <v>216359</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>24.58</v>
+      </c>
+      <c r="O4">
+        <v>4245</v>
+      </c>
+      <c r="P4">
+        <v>0.38774199999999998</v>
+      </c>
+      <c r="Q4">
+        <v>10948</v>
+      </c>
+      <c r="R4">
+        <v>8.92</v>
+      </c>
+      <c r="S4">
+        <v>19642</v>
+      </c>
+      <c r="T4">
+        <v>0.35496499999999997</v>
+      </c>
+      <c r="U4">
+        <v>55335</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0.73078782020299604</v>
+      </c>
+      <c r="AE4">
+        <v>24527</v>
+      </c>
+      <c r="AF4">
+        <v>0.39633831038717598</v>
+      </c>
+      <c r="AG4">
+        <v>61884</v>
+      </c>
+      <c r="AH4">
+        <v>32.28</v>
+      </c>
+      <c r="AI4">
+        <v>150323</v>
+      </c>
+      <c r="AJ4">
+        <v>0.40168799999999999</v>
+      </c>
+      <c r="AK4">
+        <v>374228</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -2351,101 +2361,101 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="2">
-        <v>300</v>
+      <c r="F5">
+        <v>2547</v>
       </c>
       <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
+        <v>48249</v>
+      </c>
+      <c r="H5">
         <v>3668</v>
       </c>
       <c r="I5">
-        <v>25</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.1</v>
+        <v>216359</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>25</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>24.58</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>2531</v>
       </c>
       <c r="P5">
-        <v>0.16</v>
+        <v>0.231184</v>
       </c>
       <c r="Q5">
-        <v>25</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0.1</v>
+        <v>10948</v>
+      </c>
+      <c r="R5">
+        <v>8.92</v>
       </c>
       <c r="S5">
-        <v>5</v>
+        <v>13972</v>
       </c>
       <c r="T5">
-        <v>0.16</v>
+        <v>0.252498</v>
       </c>
       <c r="U5">
-        <v>25</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0.1</v>
+        <v>55335</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>25</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
       </c>
       <c r="AA5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <v>25</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE5">
-        <v>4</v>
+        <v>12984</v>
       </c>
       <c r="AF5">
-        <v>0.14000000000000001</v>
+        <v>0.209811906146984</v>
       </c>
       <c r="AG5">
-        <v>25</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>0.1</v>
+        <v>61884</v>
+      </c>
+      <c r="AH5">
+        <v>32.28</v>
       </c>
       <c r="AI5">
-        <v>5</v>
+        <v>96993</v>
       </c>
       <c r="AJ5">
-        <v>0.16</v>
+        <v>0.25918200000000002</v>
       </c>
       <c r="AK5">
-        <v>25</v>
+        <v>374228</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -2464,101 +2474,101 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="2">
-        <v>300</v>
+      <c r="F6">
+        <v>2547</v>
       </c>
       <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6" s="2">
+        <v>21990</v>
+      </c>
+      <c r="H6">
         <v>3668</v>
       </c>
       <c r="I6">
-        <v>25</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.1</v>
+        <v>216359</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>25</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>24.58</v>
       </c>
       <c r="O6">
-        <v>6</v>
+        <v>1493</v>
       </c>
       <c r="P6">
-        <v>0.17</v>
+        <v>0.13637199999999999</v>
       </c>
       <c r="Q6">
-        <v>25</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.1</v>
+        <v>10948</v>
+      </c>
+      <c r="R6">
+        <v>8.92</v>
       </c>
       <c r="S6">
-        <v>6</v>
+        <v>4923</v>
       </c>
       <c r="T6">
-        <v>0.17</v>
+        <v>8.8967000000000004E-2</v>
       </c>
       <c r="U6">
-        <v>25</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0.1</v>
+        <v>55335</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>25</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>25</v>
-      </c>
-      <c r="AD6" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE6">
-        <v>5</v>
+        <v>7571</v>
       </c>
       <c r="AF6">
-        <v>0.15</v>
+        <v>0.122341800788572</v>
       </c>
       <c r="AG6">
-        <v>25</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>0.1</v>
+        <v>61884</v>
+      </c>
+      <c r="AH6">
+        <v>32.28</v>
       </c>
       <c r="AI6">
-        <v>6</v>
+        <v>35222</v>
       </c>
       <c r="AJ6">
-        <v>0.17</v>
+        <v>9.4118999999999994E-2</v>
       </c>
       <c r="AK6">
-        <v>25</v>
+        <v>374228</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -2577,214 +2587,214 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="2">
-        <v>300</v>
+      <c r="F7">
+        <v>2547</v>
       </c>
       <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7" s="2">
+        <v>53015</v>
+      </c>
+      <c r="H7">
         <v>3668</v>
       </c>
       <c r="I7">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.1</v>
+        <v>216359</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>25</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>24.58</v>
       </c>
       <c r="O7">
-        <v>7</v>
+        <v>2401</v>
       </c>
       <c r="P7">
-        <v>0.18</v>
+        <v>0.219309</v>
       </c>
       <c r="Q7">
-        <v>25</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.1</v>
+        <v>10948</v>
+      </c>
+      <c r="R7">
+        <v>8.92</v>
       </c>
       <c r="S7">
-        <v>7</v>
+        <v>15902</v>
       </c>
       <c r="T7">
-        <v>0.18</v>
+        <v>0.28737699999999999</v>
       </c>
       <c r="U7">
-        <v>25</v>
-      </c>
-      <c r="V7" s="2">
-        <v>0.1</v>
+        <v>55335</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <v>25</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
       </c>
       <c r="AA7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <v>25</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE7">
-        <v>6</v>
+        <v>15140</v>
       </c>
       <c r="AF7">
-        <v>0.16</v>
+        <v>0.244651283045698</v>
       </c>
       <c r="AG7">
-        <v>25</v>
-      </c>
-      <c r="AH7" s="2">
-        <v>0.1</v>
+        <v>61884</v>
+      </c>
+      <c r="AH7">
+        <v>32.28</v>
       </c>
       <c r="AI7">
-        <v>7</v>
+        <v>83359</v>
       </c>
       <c r="AJ7">
-        <v>0.18</v>
+        <v>0.222749</v>
       </c>
       <c r="AK7">
-        <v>25</v>
+        <v>374228</v>
       </c>
     </row>
     <row r="8" spans="1:37" s="2" customFormat="1">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>22</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>11002</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="2">
-        <v>300</v>
-      </c>
-      <c r="G8" s="2">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="F8">
+        <v>2547</v>
+      </c>
+      <c r="G8">
+        <v>434281</v>
+      </c>
+      <c r="H8">
         <v>3668</v>
       </c>
-      <c r="I8" s="2">
-        <v>26</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>8</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="M8" s="2">
-        <v>26</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O8" s="2">
-        <v>8</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>26</v>
-      </c>
-      <c r="R8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="S8" s="2">
-        <v>8</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="U8" s="2">
-        <v>26</v>
-      </c>
-      <c r="V8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="W8" s="2">
-        <v>8</v>
-      </c>
-      <c r="X8" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>26</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>8</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>26</v>
-      </c>
-      <c r="AD8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AE8" s="2">
-        <v>7</v>
-      </c>
-      <c r="AF8" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>16</v>
-      </c>
-      <c r="AH8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AI8" s="2">
-        <v>8</v>
-      </c>
-      <c r="AJ8" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="AK8" s="2">
-        <v>26</v>
+      <c r="I8">
+        <v>720125</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>6671</v>
+      </c>
+      <c r="L8">
+        <v>0.82155199999999995</v>
+      </c>
+      <c r="M8">
+        <v>8120</v>
+      </c>
+      <c r="N8">
+        <v>24.58</v>
+      </c>
+      <c r="O8">
+        <v>6874</v>
+      </c>
+      <c r="P8">
+        <v>0.82126600000000005</v>
+      </c>
+      <c r="Q8">
+        <v>8370</v>
+      </c>
+      <c r="R8">
+        <v>8.92</v>
+      </c>
+      <c r="S8">
+        <v>37546</v>
+      </c>
+      <c r="T8">
+        <v>0.736788</v>
+      </c>
+      <c r="U8">
+        <v>50959</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0.73078782020299604</v>
+      </c>
+      <c r="AE8">
+        <v>261889</v>
+      </c>
+      <c r="AF8">
+        <v>0.57139833744245405</v>
+      </c>
+      <c r="AG8">
+        <v>458330</v>
+      </c>
+      <c r="AH8">
+        <v>32.229999999999997</v>
+      </c>
+      <c r="AI8">
+        <v>519171</v>
+      </c>
+      <c r="AJ8">
+        <v>0.62079600000000001</v>
+      </c>
+      <c r="AK8">
+        <v>836299</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -2795,109 +2805,109 @@
         <v>11001</v>
       </c>
       <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="2">
-        <v>300</v>
+      <c r="F9">
+        <v>2547</v>
       </c>
       <c r="G9">
-        <v>9</v>
-      </c>
-      <c r="H9" s="2">
+        <v>194345</v>
+      </c>
+      <c r="H9">
         <v>3668</v>
       </c>
       <c r="I9">
-        <v>26</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.1</v>
+        <v>720125</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>9</v>
+        <v>1090</v>
       </c>
       <c r="L9">
-        <v>0.2</v>
+        <v>0.13423599999999999</v>
       </c>
       <c r="M9">
-        <v>26</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0.1</v>
+        <v>8120</v>
+      </c>
+      <c r="N9">
+        <v>24.58</v>
       </c>
       <c r="O9">
-        <v>9</v>
+        <v>1085</v>
       </c>
       <c r="P9">
-        <v>0.2</v>
+        <v>0.12963</v>
       </c>
       <c r="Q9">
-        <v>26</v>
-      </c>
-      <c r="R9" s="2">
-        <v>0.1</v>
+        <v>8370</v>
+      </c>
+      <c r="R9">
+        <v>8.92</v>
       </c>
       <c r="S9">
-        <v>9</v>
+        <v>9268</v>
       </c>
       <c r="T9">
-        <v>0.2</v>
+        <v>0.18187200000000001</v>
       </c>
       <c r="U9">
-        <v>26</v>
-      </c>
-      <c r="V9" s="2">
-        <v>0.1</v>
+        <v>50959</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="Y9">
-        <v>26</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
       </c>
       <c r="AA9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AB9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <v>26</v>
-      </c>
-      <c r="AD9" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE9">
-        <v>8</v>
+        <v>141983</v>
       </c>
       <c r="AF9">
-        <v>0.18</v>
+        <v>0.30978334387886403</v>
       </c>
       <c r="AG9">
-        <v>16</v>
-      </c>
-      <c r="AH9" s="2">
-        <v>0.1</v>
+        <v>458330</v>
+      </c>
+      <c r="AH9">
+        <v>32.229999999999997</v>
       </c>
       <c r="AI9">
-        <v>9</v>
+        <v>215637</v>
       </c>
       <c r="AJ9">
-        <v>0.2</v>
+        <v>0.25784699999999999</v>
       </c>
       <c r="AK9">
-        <v>26</v>
+        <v>836299</v>
       </c>
     </row>
     <row r="10" spans="1:37">
@@ -2908,222 +2918,222 @@
         <v>11003</v>
       </c>
       <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="2">
-        <v>300</v>
+      <c r="F10">
+        <v>2547</v>
       </c>
       <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10" s="2">
+        <v>91499</v>
+      </c>
+      <c r="H10">
         <v>3668</v>
       </c>
       <c r="I10">
-        <v>26</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.1</v>
+        <v>720125</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>10</v>
+        <v>359</v>
       </c>
       <c r="L10">
-        <v>0.21</v>
+        <v>4.4212000000000001E-2</v>
       </c>
       <c r="M10">
-        <v>26</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0.1</v>
+        <v>8120</v>
+      </c>
+      <c r="N10">
+        <v>24.58</v>
       </c>
       <c r="O10">
-        <v>10</v>
+        <v>411</v>
       </c>
       <c r="P10">
-        <v>0.21</v>
+        <v>4.9104000000000002E-2</v>
       </c>
       <c r="Q10">
-        <v>26</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0.1</v>
+        <v>8370</v>
+      </c>
+      <c r="R10">
+        <v>8.92</v>
       </c>
       <c r="S10">
-        <v>10</v>
+        <v>4145</v>
       </c>
       <c r="T10">
-        <v>0.21</v>
+        <v>8.1339999999999996E-2</v>
       </c>
       <c r="U10">
-        <v>26</v>
-      </c>
-      <c r="V10" s="2">
-        <v>0.1</v>
+        <v>50959</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <v>26</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
       </c>
       <c r="AA10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AB10">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <v>26</v>
-      </c>
-      <c r="AD10" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE10">
-        <v>9</v>
+        <v>54458</v>
       </c>
       <c r="AF10">
-        <v>0.19</v>
+        <v>0.11881831867868101</v>
       </c>
       <c r="AG10">
-        <v>16</v>
-      </c>
-      <c r="AH10" s="2">
-        <v>0.1</v>
+        <v>458330</v>
+      </c>
+      <c r="AH10">
+        <v>32.229999999999997</v>
       </c>
       <c r="AI10">
-        <v>10</v>
+        <v>101491</v>
       </c>
       <c r="AJ10">
-        <v>0.21</v>
+        <v>0.12135700000000001</v>
       </c>
       <c r="AK10">
-        <v>26</v>
+        <v>836299</v>
       </c>
     </row>
     <row r="11" spans="1:37" s="2" customFormat="1">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>23</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>164002</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="2">
-        <v>300</v>
-      </c>
-      <c r="G11" s="2">
-        <v>11</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="F11">
+        <v>2547</v>
+      </c>
+      <c r="G11">
+        <v>139745</v>
+      </c>
+      <c r="H11">
         <v>3668</v>
       </c>
-      <c r="I11" s="2">
-        <v>27</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K11" s="2">
-        <v>11</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="M11" s="2">
-        <v>27</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O11" s="2">
-        <v>11</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>27</v>
-      </c>
-      <c r="R11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="S11" s="2">
-        <v>11</v>
-      </c>
-      <c r="T11" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="U11" s="2">
-        <v>27</v>
-      </c>
-      <c r="V11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="W11" s="2">
-        <v>11</v>
-      </c>
-      <c r="X11" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="Y11" s="2">
-        <v>27</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>11</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="AC11" s="2">
-        <v>27</v>
-      </c>
-      <c r="AD11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AE11" s="2">
-        <v>10</v>
-      </c>
-      <c r="AF11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AG11" s="2">
-        <v>17</v>
-      </c>
-      <c r="AH11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AI11" s="2">
-        <v>11</v>
-      </c>
-      <c r="AJ11" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="AK11" s="2">
-        <v>27</v>
+      <c r="I11">
+        <v>194888</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>5661</v>
+      </c>
+      <c r="L11">
+        <v>0.70904299999999998</v>
+      </c>
+      <c r="M11">
+        <v>7984</v>
+      </c>
+      <c r="N11">
+        <v>24.58</v>
+      </c>
+      <c r="O11">
+        <v>6703</v>
+      </c>
+      <c r="P11">
+        <v>0.64995599999999998</v>
+      </c>
+      <c r="Q11">
+        <v>10313</v>
+      </c>
+      <c r="R11">
+        <v>8.92</v>
+      </c>
+      <c r="S11">
+        <v>38291</v>
+      </c>
+      <c r="T11">
+        <v>0.74009400000000003</v>
+      </c>
+      <c r="U11">
+        <v>51738</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0.73078782020299604</v>
+      </c>
+      <c r="AE11">
+        <v>37846</v>
+      </c>
+      <c r="AF11">
+        <v>0.71094997463979104</v>
+      </c>
+      <c r="AG11">
+        <v>53233</v>
+      </c>
+      <c r="AH11">
+        <v>32.159999999999997</v>
+      </c>
+      <c r="AI11">
+        <v>249590</v>
+      </c>
+      <c r="AJ11">
+        <v>0.717889</v>
+      </c>
+      <c r="AK11">
+        <v>347672</v>
       </c>
     </row>
     <row r="12" spans="1:37">
@@ -3134,244 +3144,244 @@
         <v>164001</v>
       </c>
       <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
         <v>68</v>
-      </c>
-      <c r="D12" t="s">
-        <v>69</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="2">
-        <v>300</v>
+      <c r="F12">
+        <v>2547</v>
       </c>
       <c r="G12">
-        <v>12</v>
-      </c>
-      <c r="H12" s="2">
+        <v>55143</v>
+      </c>
+      <c r="H12">
         <v>3668</v>
       </c>
       <c r="I12">
-        <v>27</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.1</v>
+        <v>194888</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>12</v>
+        <v>2323</v>
       </c>
       <c r="L12">
-        <v>0.23</v>
+        <v>0.29095700000000002</v>
       </c>
       <c r="M12">
-        <v>27</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0.1</v>
+        <v>7984</v>
+      </c>
+      <c r="N12">
+        <v>24.58</v>
       </c>
       <c r="O12">
-        <v>12</v>
+        <v>3610</v>
       </c>
       <c r="P12">
-        <v>0.23</v>
+        <v>0.35004400000000002</v>
       </c>
       <c r="Q12">
-        <v>27</v>
-      </c>
-      <c r="R12" s="2">
-        <v>0.1</v>
+        <v>10313</v>
+      </c>
+      <c r="R12">
+        <v>8.92</v>
       </c>
       <c r="S12">
-        <v>12</v>
+        <v>13447</v>
       </c>
       <c r="T12">
-        <v>0.23</v>
+        <v>0.25990600000000003</v>
       </c>
       <c r="U12">
-        <v>27</v>
-      </c>
-      <c r="V12" s="2">
-        <v>0.1</v>
+        <v>51738</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="Y12">
-        <v>27</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
       </c>
       <c r="AA12">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AB12">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="AC12">
-        <v>27</v>
-      </c>
-      <c r="AD12" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0.73078782020299604</v>
       </c>
       <c r="AE12">
-        <v>11</v>
+        <v>15387</v>
       </c>
       <c r="AF12">
-        <v>0.21</v>
+        <v>0.28905002536020802</v>
       </c>
       <c r="AG12">
-        <v>17</v>
-      </c>
-      <c r="AH12" s="2">
-        <v>0.1</v>
+        <v>53233</v>
+      </c>
+      <c r="AH12">
+        <v>32.159999999999997</v>
       </c>
       <c r="AI12">
-        <v>12</v>
+        <v>98082</v>
       </c>
       <c r="AJ12">
-        <v>0.23</v>
+        <v>0.282111</v>
       </c>
       <c r="AK12">
-        <v>27</v>
+        <v>347672</v>
       </c>
     </row>
     <row r="14" spans="1:37">
       <c r="C14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D14" s="8">
         <v>2069</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G14">
         <f>SUM(AD2*D14)</f>
-        <v>206.9</v>
+        <v>1511.9999999999989</v>
       </c>
     </row>
     <row r="15" spans="1:37">
       <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>72</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>73</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>74</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>75</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>76</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>77</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:37">
       <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
         <v>79</v>
       </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
       <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
         <v>79</v>
       </c>
-      <c r="F16" t="s">
-        <v>80</v>
-      </c>
       <c r="G16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" t="s">
         <v>79</v>
       </c>
-      <c r="H16" t="s">
-        <v>80</v>
-      </c>
       <c r="I16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" t="s">
         <v>79</v>
       </c>
-      <c r="J16" t="s">
-        <v>80</v>
-      </c>
       <c r="K16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" t="s">
         <v>79</v>
       </c>
-      <c r="L16" t="s">
-        <v>80</v>
-      </c>
       <c r="M16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" t="s">
         <v>79</v>
       </c>
-      <c r="N16" t="s">
-        <v>80</v>
-      </c>
       <c r="O16" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" t="s">
         <v>79</v>
       </c>
-      <c r="P16" t="s">
-        <v>80</v>
-      </c>
       <c r="Q16" t="s">
+        <v>78</v>
+      </c>
+      <c r="R16" t="s">
         <v>79</v>
-      </c>
-      <c r="R16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="5" customFormat="1">
       <c r="A17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="5">
         <f>SUM((F2-G14)/(H2-D14))</f>
-        <v>5.8223889931207001E-2</v>
+        <v>0.64727954971857482</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="5">
         <f>J2</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="5">
-        <f>N2</f>
-        <v>0.1</v>
+        <f>SUM(N2*0.01)</f>
+        <v>0.24579999999999999</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="5">
-        <f>R2</f>
-        <v>0.1</v>
+        <f>SUM(R2*0.01)</f>
+        <v>8.9200000000000002E-2</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="5">
         <f>V2</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="5">
         <f>Z2</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="5">
         <f>AD2</f>
-        <v>0.1</v>
+        <v>0.73078782020299604</v>
       </c>
       <c r="Q17" s="5">
-        <f>AH2</f>
-        <v>0.1</v>
+        <f>SUM(AH2*0.01)</f>
+        <v>0.33100000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -3380,67 +3390,67 @@
       </c>
       <c r="C18" s="7">
         <f>SUM(G2-AE2)</f>
-        <v>1</v>
+        <v>147854</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" ref="D18:D19" si="0">SUM(C18/SUM($C$18:$C$20))</f>
-        <v>0.1</v>
+        <v>0.53030188909332843</v>
       </c>
       <c r="E18" s="7">
         <f>K2</f>
-        <v>2</v>
+        <v>4509</v>
       </c>
       <c r="F18" s="4">
         <f>L2</f>
-        <v>0.13</v>
+        <v>0.51460899999999998</v>
       </c>
       <c r="G18" s="7">
         <f>O2</f>
-        <v>2</v>
+        <v>4285</v>
       </c>
       <c r="H18" s="4">
         <f>P2</f>
-        <v>0.13</v>
+        <v>0.48593799999999998</v>
       </c>
       <c r="I18" s="7">
         <f>S2</f>
-        <v>2</v>
+        <v>28074</v>
       </c>
       <c r="J18" s="4">
         <f>T2</f>
-        <v>0.13</v>
+        <v>0.50611099999999998</v>
       </c>
       <c r="K18" s="7">
         <f>W2</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L18" s="4">
         <f>X2</f>
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="M18" s="7">
         <f>AA2</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N18" s="4">
         <f>AB2</f>
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="O18" s="7">
         <f>AE2</f>
-        <v>1</v>
+        <v>267725</v>
       </c>
       <c r="P18" s="4">
         <f>AF2</f>
-        <v>0.11</v>
+        <v>0.53836903691816995</v>
       </c>
       <c r="Q18" s="7">
         <f>AI2</f>
-        <v>2</v>
+        <v>482862</v>
       </c>
       <c r="R18" s="4">
         <f>AJ2</f>
-        <v>0.13</v>
+        <v>0.52546899999999996</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -3449,67 +3459,67 @@
       </c>
       <c r="C19" s="7">
         <f>SUM(G3-AE3)</f>
-        <v>1</v>
+        <v>129277</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.46367252368091644</v>
       </c>
       <c r="E19" s="7">
         <f>K3</f>
-        <v>3</v>
+        <v>4228</v>
       </c>
       <c r="F19" s="4">
         <f>L3</f>
-        <v>0.14000000000000001</v>
+        <v>0.48253800000000002</v>
       </c>
       <c r="G19" s="7">
         <f>O3</f>
-        <v>3</v>
+        <v>4503</v>
       </c>
       <c r="H19" s="4">
         <f>P3</f>
-        <v>0.14000000000000001</v>
+        <v>0.51066</v>
       </c>
       <c r="I19" s="7">
         <f>S3</f>
-        <v>3</v>
+        <v>27227</v>
       </c>
       <c r="J19" s="4">
         <f>T3</f>
-        <v>0.14000000000000001</v>
+        <v>0.490842</v>
       </c>
       <c r="K19" s="7">
         <f>W3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L19" s="4">
         <f>X3</f>
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M19" s="7">
         <f>AA3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N19" s="4">
         <f>AB3</f>
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
         <f>AE3</f>
-        <v>2</v>
+        <v>224469</v>
       </c>
       <c r="P19" s="4">
         <f>AF3</f>
-        <v>0.12</v>
+        <v>0.451385411702249</v>
       </c>
       <c r="Q19" s="7">
         <f>AI3</f>
-        <v>3</v>
+        <v>428206</v>
       </c>
       <c r="R19" s="4">
         <f>AJ3</f>
-        <v>0.14000000000000001</v>
+        <v>0.46599000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -3518,112 +3528,112 @@
       </c>
       <c r="C20" s="7">
         <f>SUM(SUM(I2-AG2)-SUM(C18:C19))</f>
-        <v>8</v>
+        <v>1680</v>
       </c>
       <c r="D20" s="4">
         <f>SUM(C20/SUM($C$18:$C$20))</f>
-        <v>0.8</v>
+        <v>6.0255872257550811E-3</v>
       </c>
       <c r="E20" s="7">
         <f>SUM(M2-SUM(E18:E19))</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F20" s="4">
         <f>SUM(1-SUM(F18:F19))</f>
-        <v>0.73</v>
+        <v>2.8529999999999944E-3</v>
       </c>
       <c r="G20" s="7">
         <f>SUM(Q2-SUM(G18:G19))</f>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H20" s="4">
         <f>SUM(1-SUM(H18:H19))</f>
-        <v>0.73</v>
+        <v>3.4020000000000161E-3</v>
       </c>
       <c r="I20" s="7">
         <f>SUM(U2-SUM(I18:I19))</f>
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="J20" s="4">
         <f>SUM(1-SUM(J18:J19))</f>
-        <v>0.73</v>
+        <v>3.0470000000000219E-3</v>
       </c>
       <c r="K20" s="7">
         <f>SUM(Y2-SUM(K18:K19))</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="L20" s="4">
         <f>SUM(1-SUM(L18:L19))</f>
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M20" s="7">
         <f>SUM(AC2-SUM(M18:M19))</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="N20" s="4">
         <f>SUM(1-SUM(N18:N19))</f>
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="O20" s="7">
         <f>SUM(AG2-SUM(O18:O19))</f>
-        <v>11</v>
+        <v>5095</v>
       </c>
       <c r="P20" s="4">
         <f>SUM(1-SUM(P18:P19))</f>
-        <v>0.77</v>
+        <v>1.0245551379581053E-2</v>
       </c>
       <c r="Q20" s="7">
         <f>SUM(AK2-SUM(Q18:Q19))</f>
-        <v>19</v>
+        <v>7848</v>
       </c>
       <c r="R20" s="4">
         <f>SUM(1-SUM(R18:R19))</f>
-        <v>0.73</v>
+        <v>8.5410000000000208E-3</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="5" customFormat="1">
       <c r="A21" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="5">
         <f>SUM((F2-G14)/(H2-D14))</f>
-        <v>5.8223889931207001E-2</v>
+        <v>0.64727954971857482</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="5">
         <f>J4</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5">
-        <f>N4</f>
-        <v>0.1</v>
+        <f>SUM(N2*0.01)</f>
+        <v>0.24579999999999999</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="5">
-        <f>R4</f>
-        <v>0.1</v>
+        <f>SUM(R2*0.01)</f>
+        <v>8.9200000000000002E-2</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="5">
         <f>V4</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="5">
         <f>Z4</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="5">
         <f>AD4</f>
-        <v>0.1</v>
+        <v>0.73078782020299604</v>
       </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="5">
-        <f>AH4</f>
-        <v>0.1</v>
+        <f>SUM(AH12*0.01)</f>
+        <v>0.3216</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -3632,67 +3642,67 @@
       </c>
       <c r="C22" s="7">
         <f>SUM(G4-AE4)</f>
-        <v>1</v>
-      </c>
-      <c r="D22" s="4" t="e">
+        <v>64282</v>
+      </c>
+      <c r="D22" s="4">
         <f t="shared" ref="D22:D25" si="1">SUM(C22/SUM($C$22:$C$26))</f>
-        <v>#DIV/0!</v>
+        <v>0.41613206020391647</v>
       </c>
       <c r="E22" s="7">
         <f>K4</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <f>L4</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G22" s="7">
         <f>O4</f>
-        <v>4</v>
+        <v>4245</v>
       </c>
       <c r="H22" s="4">
         <f>P4</f>
-        <v>0.15</v>
+        <v>0.38774199999999998</v>
       </c>
       <c r="I22" s="7">
         <f>S4</f>
-        <v>4</v>
+        <v>19642</v>
       </c>
       <c r="J22" s="4">
         <f>T4</f>
-        <v>0.15</v>
+        <v>0.35496499999999997</v>
       </c>
       <c r="K22" s="7">
         <f>W4</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L22" s="4">
         <f>X4</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="M22" s="7">
         <f>AA4</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N22" s="4">
         <f>AB4</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="O22" s="7">
         <f>AE4</f>
-        <v>3</v>
+        <v>24527</v>
       </c>
       <c r="P22" s="4">
         <f>AF4</f>
-        <v>0.13</v>
+        <v>0.39633831038717598</v>
       </c>
       <c r="Q22" s="7">
         <f>AI4</f>
-        <v>4</v>
+        <v>150323</v>
       </c>
       <c r="R22" s="4">
         <f>AJ4</f>
-        <v>0.15</v>
+        <v>0.40168799999999999</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -3701,67 +3711,67 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" ref="C23:C25" si="2">SUM(G5-AE5)</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="4" t="e">
+        <v>35265</v>
+      </c>
+      <c r="D23" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.2282893672115229</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" ref="E23:E25" si="3">K5</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" ref="F23:F25" si="4">L5</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" ref="G23:G25" si="5">O5</f>
-        <v>5</v>
+        <v>2531</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" ref="H23:H25" si="6">P5</f>
-        <v>0.16</v>
+        <v>0.231184</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" ref="I23:I25" si="7">S5</f>
-        <v>5</v>
+        <v>13972</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" ref="J23:J25" si="8">T5</f>
-        <v>0.16</v>
+        <v>0.252498</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" ref="K23:K25" si="9">W5</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" ref="L23:L25" si="10">X5</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="M23" s="7">
         <f t="shared" ref="M23:M25" si="11">AA5</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N23" s="4">
         <f t="shared" ref="N23:N25" si="12">AB5</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="O23" s="7">
         <f t="shared" ref="O23:O25" si="13">AE5</f>
-        <v>4</v>
+        <v>12984</v>
       </c>
       <c r="P23" s="4">
         <f t="shared" ref="P23:P25" si="14">AF5</f>
-        <v>0.14000000000000001</v>
+        <v>0.209811906146984</v>
       </c>
       <c r="Q23" s="7">
         <f t="shared" ref="Q23:Q25" si="15">AI5</f>
-        <v>5</v>
+        <v>96993</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" ref="R23:R25" si="16">AJ5</f>
-        <v>0.16</v>
+        <v>0.25918200000000002</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -3770,67 +3780,67 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="e">
+        <v>14419</v>
+      </c>
+      <c r="D24" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>9.3341964719210233E-2</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="4"/>
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>1493</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="6"/>
-        <v>0.17</v>
+        <v>0.13637199999999999</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>4923</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="8"/>
-        <v>0.17</v>
+        <v>8.8967000000000004E-2</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="10"/>
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="M24" s="7">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N24" s="4">
         <f t="shared" si="12"/>
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="O24" s="7">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>7571</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="14"/>
-        <v>0.15</v>
+        <v>0.122341800788572</v>
       </c>
       <c r="Q24" s="7">
         <f t="shared" si="15"/>
-        <v>6</v>
+        <v>35222</v>
       </c>
       <c r="R24" s="4">
         <f t="shared" si="16"/>
-        <v>0.17</v>
+        <v>9.4118999999999994E-2</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -3839,67 +3849,67 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D25" s="4" t="e">
+        <v>37875</v>
+      </c>
+      <c r="D25" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.24518530506554459</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="4"/>
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>2401</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="6"/>
-        <v>0.18</v>
+        <v>0.219309</v>
       </c>
       <c r="I25" s="7">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>15902</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="8"/>
-        <v>0.18</v>
+        <v>0.28737699999999999</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="10"/>
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="M25" s="7">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="12"/>
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="O25" s="7">
         <f t="shared" si="13"/>
-        <v>6</v>
+        <v>15140</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="14"/>
-        <v>0.16</v>
+        <v>0.244651283045698</v>
       </c>
       <c r="Q25" s="7">
         <f t="shared" si="15"/>
-        <v>7</v>
+        <v>83359</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="16"/>
-        <v>0.18</v>
+        <v>0.222749</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -3908,502 +3918,502 @@
       </c>
       <c r="C26" s="7">
         <f>SUM((I4-AG4)-SUM(C22:C25))</f>
-        <v>-4</v>
-      </c>
-      <c r="D26" s="4" t="e">
+        <v>2634</v>
+      </c>
+      <c r="D26" s="4">
         <f>SUM(C26/SUM($C$22:$C$26))</f>
-        <v>#DIV/0!</v>
+        <v>1.7051302799805795E-2</v>
       </c>
       <c r="E26" s="7">
         <f>SUM(M4-SUM(E22:E25))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F26" s="4">
         <f>SUM(1-SUM(F22:F25))</f>
-        <v>0.34000000000000008</v>
+        <v>1</v>
       </c>
       <c r="G26" s="7">
         <f>SUM(Q4-SUM(G22:G25))</f>
-        <v>3</v>
+        <v>278</v>
       </c>
       <c r="H26" s="4">
         <f>SUM(1-SUM(H22:H25))</f>
-        <v>0.34000000000000008</v>
+        <v>2.5392999999999999E-2</v>
       </c>
       <c r="I26" s="7">
         <f>SUM(U4-SUM(I22:I25))</f>
-        <v>3</v>
+        <v>896</v>
       </c>
       <c r="J26" s="4">
         <f>SUM(1-SUM(J22:J25))</f>
-        <v>0.34000000000000008</v>
+        <v>1.6193000000000013E-2</v>
       </c>
       <c r="K26" s="7">
         <f>SUM(Y4-SUM(K22:K25))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L26" s="4">
         <f>SUM(1-SUM(L22:L25))</f>
-        <v>0.34000000000000008</v>
+        <v>1</v>
       </c>
       <c r="M26" s="7">
         <f>SUM(AC4-SUM(M22:M25))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N26" s="4">
         <f>SUM(1-SUM(N22:N25))</f>
-        <v>0.34000000000000008</v>
+        <v>1</v>
       </c>
       <c r="O26" s="7">
         <f>SUM(AG4-SUM(O22:O25))</f>
-        <v>7</v>
+        <v>1662</v>
       </c>
       <c r="P26" s="4">
         <f>SUM(1-SUM(P22:P25))</f>
-        <v>0.41999999999999993</v>
+        <v>2.6856699631570002E-2</v>
       </c>
       <c r="Q26" s="7">
         <f>SUM(AK4-SUM(Q22:Q25))</f>
-        <v>3</v>
+        <v>8331</v>
       </c>
       <c r="R26" s="4">
         <f>SUM(1-SUM(R22:R25))</f>
-        <v>0.34000000000000008</v>
+        <v>2.2262000000000004E-2</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="5" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="5">
         <f>SUM((F2-G14)/(H2-D14))</f>
-        <v>5.8223889931207001E-2</v>
+        <v>0.64727954971857482</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
         <f>J8</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5">
-        <f>N8</f>
-        <v>0.1</v>
+        <f>SUM(N2*0.01)</f>
+        <v>0.24579999999999999</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="5">
-        <f>R8</f>
-        <v>0.1</v>
+        <f>SUM(R2*0.01)</f>
+        <v>8.9200000000000002E-2</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="5">
         <f>V8</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="5">
         <f>Z8</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" s="5">
         <f>AD8</f>
-        <v>0.1</v>
+        <v>0.73078782020299604</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="5">
-        <f>AH8</f>
-        <v>0.1</v>
+        <f>SUM(AH12*0.01)</f>
+        <v>0.3216</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7">
         <f>SUM(G8-AE8)</f>
-        <v>1</v>
+        <v>172392</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" ref="D28:D29" si="17">SUM(C28/SUM($C$28:$C$30))</f>
-        <v>0.33333333333333331</v>
+        <v>0.65849997135163008</v>
       </c>
       <c r="E28" s="7">
         <f>K8</f>
-        <v>8</v>
+        <v>6671</v>
       </c>
       <c r="F28" s="4">
         <f>L8</f>
-        <v>0.19</v>
+        <v>0.82155199999999995</v>
       </c>
       <c r="G28" s="7">
         <f>O8</f>
-        <v>8</v>
+        <v>6874</v>
       </c>
       <c r="H28" s="4">
         <f>P8</f>
-        <v>0.19</v>
+        <v>0.82126600000000005</v>
       </c>
       <c r="I28" s="7">
         <f>S8</f>
-        <v>8</v>
+        <v>37546</v>
       </c>
       <c r="J28" s="4">
         <f>T8</f>
-        <v>0.19</v>
+        <v>0.736788</v>
       </c>
       <c r="K28" s="7">
         <f>W8</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L28" s="4">
         <f>X8</f>
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="M28" s="7">
         <f>AA8</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N28" s="4">
         <f>AB8</f>
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="O28" s="7">
         <f>AE8</f>
-        <v>7</v>
+        <v>261889</v>
       </c>
       <c r="P28" s="4">
         <f>AF8</f>
-        <v>0.17</v>
+        <v>0.57139833744245405</v>
       </c>
       <c r="Q28" s="7">
         <f>AI8</f>
-        <v>8</v>
+        <v>519171</v>
       </c>
       <c r="R28" s="4">
         <f>AJ8</f>
-        <v>0.19</v>
+        <v>0.62079600000000001</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="7">
         <f>SUM(G9-AE9)</f>
-        <v>1</v>
+        <v>52362</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="17"/>
-        <v>0.33333333333333331</v>
+        <v>0.20001145934796311</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" ref="E29:E30" si="18">K9</f>
-        <v>9</v>
+        <v>1090</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" ref="F29:F30" si="19">L9</f>
-        <v>0.2</v>
+        <v>0.13423599999999999</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" ref="G29:G30" si="20">O9</f>
-        <v>9</v>
+        <v>1085</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" ref="H29:H30" si="21">P9</f>
-        <v>0.2</v>
+        <v>0.12963</v>
       </c>
       <c r="I29" s="7">
         <f t="shared" ref="I29:I30" si="22">S9</f>
-        <v>9</v>
+        <v>9268</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" ref="J29:J30" si="23">T9</f>
-        <v>0.2</v>
+        <v>0.18187200000000001</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" ref="K29:K30" si="24">W9</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" ref="L29:L30" si="25">X9</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="M29" s="7">
         <f t="shared" ref="M29:M30" si="26">AA9</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="N29" s="4">
         <f t="shared" ref="N29:N30" si="27">AB9</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O29" s="7">
         <f t="shared" ref="O29:O30" si="28">AE9</f>
-        <v>8</v>
+        <v>141983</v>
       </c>
       <c r="P29" s="4">
         <f t="shared" ref="P29:P30" si="29">AF9</f>
-        <v>0.18</v>
+        <v>0.30978334387886403</v>
       </c>
       <c r="Q29" s="7">
         <f t="shared" ref="Q29:Q30" si="30">AI9</f>
-        <v>9</v>
+        <v>215637</v>
       </c>
       <c r="R29" s="4">
         <f t="shared" ref="R29:R30" si="31">AJ9</f>
-        <v>0.2</v>
+        <v>0.25784699999999999</v>
       </c>
     </row>
     <row r="30" spans="1:18">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="7">
         <f>SUM(G10-AE10)</f>
-        <v>1</v>
+        <v>37041</v>
       </c>
       <c r="D30" s="4">
         <f>SUM(C30/SUM($C$28:$C$30))</f>
-        <v>0.33333333333333331</v>
+        <v>0.14148856930040682</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="18"/>
-        <v>10</v>
+        <v>359</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="19"/>
-        <v>0.21</v>
+        <v>4.4212000000000001E-2</v>
       </c>
       <c r="G30" s="7">
         <f t="shared" si="20"/>
-        <v>10</v>
+        <v>411</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="21"/>
-        <v>0.21</v>
+        <v>4.9104000000000002E-2</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="22"/>
-        <v>10</v>
+        <v>4145</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="23"/>
-        <v>0.21</v>
+        <v>8.1339999999999996E-2</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="24"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="25"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="M30" s="7">
         <f t="shared" si="26"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N30" s="4">
         <f t="shared" si="27"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="O30" s="7">
         <f t="shared" si="28"/>
-        <v>9</v>
+        <v>54458</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" si="29"/>
-        <v>0.19</v>
+        <v>0.11881831867868101</v>
       </c>
       <c r="Q30" s="7">
         <f t="shared" si="30"/>
-        <v>10</v>
+        <v>101491</v>
       </c>
       <c r="R30" s="4">
         <f t="shared" si="31"/>
-        <v>0.21</v>
+        <v>0.12135700000000001</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="5" customFormat="1">
       <c r="A31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="5">
         <f>SUM((F2-G14)/(H2-D14))</f>
-        <v>5.8223889931207001E-2</v>
+        <v>0.64727954971857482</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
         <f>J11</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="5">
-        <f>N11</f>
-        <v>0.1</v>
+        <f>SUM(N2*0.01)</f>
+        <v>0.24579999999999999</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="5">
-        <f>R11</f>
-        <v>0.1</v>
+        <f>SUM(R2*0.01)</f>
+        <v>8.9200000000000002E-2</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="5">
         <f>V11</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="6"/>
       <c r="M31" s="5">
         <f>Z11</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N31" s="6"/>
       <c r="O31" s="5">
         <f>AD11</f>
-        <v>0.1</v>
+        <v>0.73078782020299604</v>
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="5">
-        <f>AH11</f>
-        <v>0.1</v>
+        <f>SUM(AH12*0.01)</f>
+        <v>0.3216</v>
       </c>
     </row>
     <row r="32" spans="1:18">
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="7">
         <f>SUM(G11-AE11)</f>
-        <v>1</v>
+        <v>101899</v>
       </c>
       <c r="D32" s="4">
         <f>SUM(C32/SUM($C$32:$C$33))</f>
-        <v>0.5</v>
+        <v>0.71934629910698533</v>
       </c>
       <c r="E32" s="7">
         <f>K11</f>
-        <v>11</v>
+        <v>5661</v>
       </c>
       <c r="F32" s="4">
         <f>L11</f>
-        <v>0.22</v>
+        <v>0.70904299999999998</v>
       </c>
       <c r="G32" s="7">
         <f>O11</f>
-        <v>11</v>
+        <v>6703</v>
       </c>
       <c r="H32" s="4">
         <f>P11</f>
-        <v>0.22</v>
+        <v>0.64995599999999998</v>
       </c>
       <c r="I32" s="7">
         <f>S11</f>
-        <v>11</v>
+        <v>38291</v>
       </c>
       <c r="J32" s="4">
         <f>T11</f>
-        <v>0.22</v>
+        <v>0.74009400000000003</v>
       </c>
       <c r="K32" s="7">
         <f>W11</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L32" s="4">
         <f>X11</f>
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="M32" s="7">
         <f>AA11</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N32" s="4">
         <f>AB11</f>
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="O32" s="7">
         <f>AE11</f>
-        <v>10</v>
+        <v>37846</v>
       </c>
       <c r="P32" s="4">
         <f>AF11</f>
-        <v>0.2</v>
+        <v>0.71094997463979104</v>
       </c>
       <c r="Q32" s="7">
         <f>AI11</f>
-        <v>11</v>
+        <v>249590</v>
       </c>
       <c r="R32" s="4">
         <f>AJ11</f>
-        <v>0.22</v>
+        <v>0.717889</v>
       </c>
     </row>
     <row r="33" spans="2:18">
       <c r="B33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="7">
         <f>SUM(G12-AE12)</f>
-        <v>1</v>
+        <v>39756</v>
       </c>
       <c r="D33" s="4">
         <f>SUM(C33/SUM($C$32:$C$33))</f>
-        <v>0.5</v>
+        <v>0.28065370089301472</v>
       </c>
       <c r="E33" s="7">
         <f>K12</f>
-        <v>12</v>
+        <v>2323</v>
       </c>
       <c r="F33" s="4">
         <f>L12</f>
-        <v>0.23</v>
+        <v>0.29095700000000002</v>
       </c>
       <c r="G33" s="7">
         <f>O12</f>
-        <v>12</v>
+        <v>3610</v>
       </c>
       <c r="H33" s="4">
         <f>P12</f>
-        <v>0.23</v>
+        <v>0.35004400000000002</v>
       </c>
       <c r="I33" s="7">
         <f>S12</f>
-        <v>12</v>
+        <v>13447</v>
       </c>
       <c r="J33" s="4">
         <f>T12</f>
-        <v>0.23</v>
+        <v>0.25990600000000003</v>
       </c>
       <c r="K33" s="7">
         <f>W12</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L33" s="4">
         <f>X12</f>
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="M33" s="7">
         <f>AA12</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N33" s="4">
         <f>AB12</f>
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="O33" s="7">
         <f>AE12</f>
-        <v>11</v>
+        <v>15387</v>
       </c>
       <c r="P33" s="4">
         <f>AF12</f>
-        <v>0.21</v>
+        <v>0.28905002536020802</v>
       </c>
       <c r="Q33" s="7">
         <f>AI12</f>
-        <v>12</v>
+        <v>98082</v>
       </c>
       <c r="R33" s="4">
         <f>AJ12</f>
-        <v>0.23</v>
+        <v>0.282111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>